<commit_message>
check on the photoperiod
</commit_message>
<xml_diff>
--- a/Prototypes/Rice/Observed_vv16.xlsx
+++ b/Prototypes/Rice/Observed_vv16.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2020_Try_model\APSIMXRICE\Prototypes\Rice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C088224-DD12-411A-A546-86DCCF14257F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9FFB1CD-FA96-4958-8991-02C32A3A8BE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12420" xr2:uid="{4E4677B1-1A06-474B-9D94-864A1DB18DBC}"/>
+    <workbookView xWindow="52680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{4E4677B1-1A06-474B-9D94-864A1DB18DBC}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
@@ -762,8 +762,8 @@
   <dimension ref="A1:V406"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M1" sqref="M1"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V319" sqref="V319"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6606,7 +6606,7 @@
         <v>443.67567567567556</v>
       </c>
     </row>
-    <row r="235" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
         <v>86</v>
       </c>
@@ -6695,7 +6695,7 @@
         <v>370.00000000000006</v>
       </c>
     </row>
-    <row r="239" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
         <v>87</v>
       </c>
@@ -6775,7 +6775,7 @@
         <v>506.19459183966472</v>
       </c>
     </row>
-    <row r="243" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
         <v>88</v>
       </c>
@@ -6855,7 +6855,7 @@
         <v>487.41484352824079</v>
       </c>
     </row>
-    <row r="247" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
         <v>89</v>
       </c>
@@ -6935,7 +6935,7 @@
         <v>464.75639619883043</v>
       </c>
     </row>
-    <row r="251" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
         <v>90</v>
       </c>
@@ -7015,7 +7015,7 @@
         <v>550.27810936931712</v>
       </c>
     </row>
-    <row r="255" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
         <v>91</v>
       </c>
@@ -7095,7 +7095,7 @@
         <v>448.78598617814833</v>
       </c>
     </row>
-    <row r="259" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
         <v>92</v>
       </c>
@@ -7175,7 +7175,7 @@
         <v>464.7976378403111</v>
       </c>
     </row>
-    <row r="263" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
         <v>93</v>
       </c>
@@ -7255,7 +7255,7 @@
         <v>380.8539124668435</v>
       </c>
     </row>
-    <row r="267" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
         <v>94</v>
       </c>
@@ -7335,7 +7335,7 @@
         <v>459.2430335968379</v>
       </c>
     </row>
-    <row r="271" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
         <v>95</v>
       </c>
@@ -7707,7 +7707,7 @@
         <v>245.86765005354539</v>
       </c>
     </row>
-    <row r="298" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A298" t="s">
         <v>86</v>
       </c>
@@ -7718,7 +7718,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="299" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A299" t="s">
         <v>87</v>
       </c>
@@ -7729,7 +7729,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="300" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A300" t="s">
         <v>88</v>
       </c>
@@ -7743,7 +7743,7 @@
         <v>1.0897247358851685</v>
       </c>
     </row>
-    <row r="301" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A301" t="s">
         <v>89</v>
       </c>
@@ -7757,7 +7757,7 @@
         <v>0.4330127018922193</v>
       </c>
     </row>
-    <row r="302" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A302" t="s">
         <v>90</v>
       </c>
@@ -7771,7 +7771,7 @@
         <v>0.4330127018922193</v>
       </c>
     </row>
-    <row r="303" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A303" t="s">
         <v>91</v>
       </c>
@@ -7785,7 +7785,7 @@
         <v>0.4330127018922193</v>
       </c>
     </row>
-    <row r="304" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A304" t="s">
         <v>92</v>
       </c>
@@ -7799,7 +7799,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="305" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A305" t="s">
         <v>93</v>
       </c>
@@ -7813,7 +7813,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="306" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A306" t="s">
         <v>94</v>
       </c>
@@ -7827,7 +7827,7 @@
         <v>2.3452078799117149</v>
       </c>
     </row>
-    <row r="307" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A307" t="s">
         <v>95</v>
       </c>
@@ -7838,7 +7838,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="308" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A308" t="s">
         <v>96</v>
       </c>
@@ -7852,7 +7852,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="309" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A309" t="s">
         <v>97</v>
       </c>
@@ -7866,7 +7866,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="310" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A310" t="s">
         <v>98</v>
       </c>
@@ -7880,7 +7880,7 @@
         <v>4.4930501889028571</v>
       </c>
     </row>
-    <row r="311" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A311" t="s">
         <v>99</v>
       </c>
@@ -7894,7 +7894,7 @@
         <v>0.4330127018922193</v>
       </c>
     </row>
-    <row r="312" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A312" t="s">
         <v>100</v>
       </c>
@@ -7908,7 +7908,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="313" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A313" t="s">
         <v>101</v>
       </c>
@@ -7922,7 +7922,7 @@
         <v>0.4330127018922193</v>
       </c>
     </row>
-    <row r="314" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A314" t="s">
         <v>102</v>
       </c>
@@ -7936,7 +7936,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="315" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A315" t="s">
         <v>103</v>
       </c>
@@ -7950,7 +7950,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="316" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A316" t="s">
         <v>104</v>
       </c>
@@ -7964,7 +7964,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="317" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A317" t="s">
         <v>105</v>
       </c>
@@ -7978,7 +7978,7 @@
         <v>0.82915619758884995</v>
       </c>
     </row>
-    <row r="318" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A318" t="s">
         <v>106</v>
       </c>
@@ -7992,7 +7992,7 @@
         <v>0.70710678118654757</v>
       </c>
     </row>
-    <row r="319" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A319" t="s">
         <v>107</v>
       </c>
@@ -8006,7 +8006,7 @@
         <v>1.0897247358851685</v>
       </c>
     </row>
-    <row r="320" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A320" t="s">
         <v>108</v>
       </c>
@@ -8020,7 +8020,7 @@
         <v>0.82915619758884995</v>
       </c>
     </row>
-    <row r="321" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A321" t="s">
         <v>109</v>
       </c>
@@ -8034,7 +8034,7 @@
         <v>0.82915619758884995</v>
       </c>
     </row>
-    <row r="322" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A322" t="s">
         <v>110</v>
       </c>
@@ -8048,7 +8048,7 @@
         <v>3.7666297933298409</v>
       </c>
     </row>
-    <row r="323" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A323" t="s">
         <v>111</v>
       </c>
@@ -8062,7 +8062,7 @@
         <v>4.3301270189221936</v>
       </c>
     </row>
-    <row r="324" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A324" t="s">
         <v>112</v>
       </c>
@@ -8076,7 +8076,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="325" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A325" t="s">
         <v>113</v>
       </c>
@@ -8090,7 +8090,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="326" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A326" t="s">
         <v>114</v>
       </c>
@@ -8104,7 +8104,7 @@
         <v>1.8708286933869707</v>
       </c>
     </row>
-    <row r="327" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A327" t="s">
         <v>115</v>
       </c>
@@ -8118,7 +8118,7 @@
         <v>2.9154759474226504</v>
       </c>
     </row>
-    <row r="328" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A328" t="s">
         <v>116</v>
       </c>
@@ -8132,7 +8132,7 @@
         <v>3.5355339059327378</v>
       </c>
     </row>
-    <row r="329" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A329" t="s">
         <v>117</v>
       </c>
@@ -8146,7 +8146,7 @@
         <v>2.3452078799117149</v>
       </c>
     </row>
-    <row r="330" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A330" t="s">
         <v>118</v>
       </c>
@@ -8160,7 +8160,7 @@
         <v>3.2691742076555053</v>
       </c>
     </row>
-    <row r="331" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A331" t="s">
         <v>119</v>
       </c>
@@ -8174,7 +8174,7 @@
         <v>4.1457809879442502</v>
       </c>
     </row>
-    <row r="332" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A332" t="s">
         <v>120</v>
       </c>
@@ -8188,7 +8188,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="333" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A333" t="s">
         <v>121</v>
       </c>
@@ -8202,7 +8202,7 @@
         <v>5.196152422706632</v>
       </c>
     </row>
-    <row r="334" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A334" t="s">
         <v>86</v>
       </c>
@@ -8213,7 +8213,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="335" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A335" t="s">
         <v>87</v>
       </c>
@@ -8224,7 +8224,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="336" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A336" t="s">
         <v>88</v>
       </c>
@@ -8238,7 +8238,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="337" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A337" t="s">
         <v>89</v>
       </c>
@@ -8252,7 +8252,7 @@
         <v>0.70710678118654757</v>
       </c>
     </row>
-    <row r="338" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A338" t="s">
         <v>90</v>
       </c>
@@ -8266,7 +8266,7 @@
         <v>0.4330127018922193</v>
       </c>
     </row>
-    <row r="339" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A339" t="s">
         <v>91</v>
       </c>
@@ -8280,7 +8280,7 @@
         <v>1.0897247358851685</v>
       </c>
     </row>
-    <row r="340" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A340" t="s">
         <v>92</v>
       </c>
@@ -8291,7 +8291,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="341" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A341" t="s">
         <v>93</v>
       </c>
@@ -8302,7 +8302,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="342" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A342" t="s">
         <v>94</v>
       </c>
@@ -8313,7 +8313,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="343" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A343" t="s">
         <v>95</v>
       </c>
@@ -8324,7 +8324,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="344" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A344" t="s">
         <v>96</v>
       </c>
@@ -8338,7 +8338,7 @@
         <v>4.636809247747852</v>
       </c>
     </row>
-    <row r="345" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A345" t="s">
         <v>97</v>
       </c>
@@ -8352,7 +8352,7 @@
         <v>0.70710678118654757</v>
       </c>
     </row>
-    <row r="346" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A346" t="s">
         <v>98</v>
       </c>
@@ -8366,7 +8366,7 @@
         <v>0.4330127018922193</v>
       </c>
     </row>
-    <row r="347" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A347" t="s">
         <v>99</v>
       </c>
@@ -8380,7 +8380,7 @@
         <v>1.299038105676658</v>
       </c>
     </row>
-    <row r="348" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A348" t="s">
         <v>100</v>
       </c>
@@ -8391,7 +8391,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="349" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A349" t="s">
         <v>101</v>
       </c>
@@ -8405,7 +8405,7 @@
         <v>0.70710678118654757</v>
       </c>
     </row>
-    <row r="350" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A350" t="s">
         <v>102</v>
       </c>
@@ -8419,7 +8419,7 @@
         <v>1.2247448713915889</v>
       </c>
     </row>
-    <row r="351" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A351" t="s">
         <v>103</v>
       </c>
@@ -8433,7 +8433,7 @@
         <v>0.8660254037844386</v>
       </c>
     </row>
-    <row r="352" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A352" t="s">
         <v>104</v>
       </c>
@@ -8447,7 +8447,7 @@
         <v>0.4330127018922193</v>
       </c>
     </row>
-    <row r="353" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A353" t="s">
         <v>105</v>
       </c>
@@ -8461,7 +8461,7 @@
         <v>5.6789083458002736</v>
       </c>
     </row>
-    <row r="354" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A354" t="s">
         <v>106</v>
       </c>
@@ -8475,7 +8475,7 @@
         <v>1.1180339887498949</v>
       </c>
     </row>
-    <row r="355" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A355" t="s">
         <v>107</v>
       </c>
@@ -8489,7 +8489,7 @@
         <v>1.299038105676658</v>
       </c>
     </row>
-    <row r="356" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A356" t="s">
         <v>108</v>
       </c>
@@ -8503,7 +8503,7 @@
         <v>0.4330127018922193</v>
       </c>
     </row>
-    <row r="357" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A357" t="s">
         <v>109</v>
       </c>
@@ -8514,7 +8514,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="358" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A358" t="s">
         <v>110</v>
       </c>
@@ -8528,7 +8528,7 @@
         <v>0.8660254037844386</v>
       </c>
     </row>
-    <row r="359" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A359" t="s">
         <v>111</v>
       </c>
@@ -8539,7 +8539,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="360" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A360" t="s">
         <v>112</v>
       </c>
@@ -8553,7 +8553,7 @@
         <v>0.8660254037844386</v>
       </c>
     </row>
-    <row r="361" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A361" t="s">
         <v>113</v>
       </c>
@@ -8564,7 +8564,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="362" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A362" t="s">
         <v>114</v>
       </c>
@@ -8575,7 +8575,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="363" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A363" t="s">
         <v>115</v>
       </c>
@@ -8586,7 +8586,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="364" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A364" t="s">
         <v>116</v>
       </c>
@@ -8600,7 +8600,7 @@
         <v>1.7320508075688772</v>
       </c>
     </row>
-    <row r="365" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A365" t="s">
         <v>117</v>
       </c>
@@ -8614,7 +8614,7 @@
         <v>0.8660254037844386</v>
       </c>
     </row>
-    <row r="366" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A366" t="s">
         <v>118</v>
       </c>
@@ -8628,7 +8628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="367" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A367" t="s">
         <v>119</v>
       </c>
@@ -8639,7 +8639,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="368" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A368" t="s">
         <v>120</v>
       </c>
@@ -8653,7 +8653,7 @@
         <v>1.920286436967152</v>
       </c>
     </row>
-    <row r="369" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A369" t="s">
         <v>121</v>
       </c>
@@ -9162,10 +9162,11 @@
     <row r="406" spans="1:18" hidden="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <autoFilter ref="A1:V406" xr:uid="{C04573D9-2538-4EBF-9F26-33FC1F82F101}">
-    <filterColumn colId="12">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
+    <filterColumn colId="1">
+      <filters>
+        <dateGroupItem year="2018" month="5" dateTimeGrouping="month"/>
+        <dateGroupItem year="2018" month="12" dateTimeGrouping="month"/>
+      </filters>
     </filterColumn>
     <filterColumn colId="16">
       <filters blank="1"/>

</xml_diff>